<commit_message>
fixed logic to move files according to the months. added suppliers to the list.
</commit_message>
<xml_diff>
--- a/Supplier-Payment-Method.xlsx
+++ b/Supplier-Payment-Method.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scott/Learning/Coding/Python3/sort-invoice/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scott/Projects/Python Projects/sort-invoice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F08827-7386-6145-8C3E-04BE187402F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F469627A-9270-6C45-8D74-BAA3D007C373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="49720" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18700" yWindow="500" windowWidth="23360" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="96">
   <si>
     <t>Suppliers</t>
   </si>
@@ -133,12 +133,6 @@
     <t>DFI</t>
   </si>
   <si>
-    <t>coles</t>
-  </si>
-  <si>
-    <t>fuel</t>
-  </si>
-  <si>
     <t>feeder</t>
   </si>
   <si>
@@ -148,18 +142,12 @@
     <t>kmall09</t>
   </si>
   <si>
-    <t>super</t>
-  </si>
-  <si>
     <t>seek business</t>
   </si>
   <si>
     <t>food packaging</t>
   </si>
   <si>
-    <t>google</t>
-  </si>
-  <si>
     <t>coursera</t>
   </si>
   <si>
@@ -184,9 +172,6 @@
     <t>telstra</t>
   </si>
   <si>
-    <t>petrol</t>
-  </si>
-  <si>
     <t>lululemon</t>
   </si>
   <si>
@@ -205,9 +190,6 @@
     <t>Tongli</t>
   </si>
   <si>
-    <t>post</t>
-  </si>
-  <si>
     <t>Food Dairy</t>
   </si>
   <si>
@@ -274,10 +256,58 @@
     <t>nova</t>
   </si>
   <si>
-    <t>rent</t>
-  </si>
-  <si>
     <t>bombora</t>
+  </si>
+  <si>
+    <t>1Password</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
+    <t>Expedia Hotel</t>
+  </si>
+  <si>
+    <t>Agoda</t>
+  </si>
+  <si>
+    <t>Kmall</t>
+  </si>
+  <si>
+    <t>WL Filter</t>
+  </si>
+  <si>
+    <t>Cleanaway</t>
+  </si>
+  <si>
+    <t>Victoria Basement</t>
+  </si>
+  <si>
+    <t>Premier Tazze</t>
+  </si>
+  <si>
+    <t>Auspost</t>
+  </si>
+  <si>
+    <t>Coles</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>New Yenyen</t>
+  </si>
+  <si>
+    <t>New renren</t>
+  </si>
+  <si>
+    <t>Crocs</t>
+  </si>
+  <si>
+    <t>Metro Petrol</t>
+  </si>
+  <si>
+    <t>Medco Petrol</t>
   </si>
 </sst>
 </file>
@@ -640,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B83"/>
+  <dimension ref="A1:B93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1086,7 +1116,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="B55" t="s">
         <v>3</v>
@@ -1094,15 +1124,15 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>3</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B57" t="s">
         <v>3</v>
@@ -1110,7 +1140,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B58" t="s">
         <v>3</v>
@@ -1118,7 +1148,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="B59" t="s">
         <v>3</v>
@@ -1126,7 +1156,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B60" t="s">
         <v>3</v>
@@ -1134,34 +1164,34 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>3</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>3</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>3</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>3</v>
+        <v>61</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
@@ -1169,7 +1199,7 @@
         <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>3</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -1177,79 +1207,79 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>75</v>
+      </c>
+      <c r="B75" t="s">
         <v>76</v>
-      </c>
-      <c r="B75" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
@@ -1257,7 +1287,7 @@
         <v>77</v>
       </c>
       <c r="B76" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
@@ -1265,7 +1295,7 @@
         <v>78</v>
       </c>
       <c r="B77" t="s">
-        <v>67</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
@@ -1273,7 +1303,7 @@
         <v>79</v>
       </c>
       <c r="B78" t="s">
-        <v>67</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
@@ -1281,7 +1311,7 @@
         <v>80</v>
       </c>
       <c r="B79" t="s">
-        <v>67</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
@@ -1289,30 +1319,110 @@
         <v>81</v>
       </c>
       <c r="B80" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B81" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B82" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>84</v>
+      </c>
+      <c r="B83" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>85</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B84" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>86</v>
+      </c>
+      <c r="B85" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>87</v>
+      </c>
+      <c r="B86" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>89</v>
+      </c>
+      <c r="B87" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>90</v>
+      </c>
+      <c r="B88" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>91</v>
+      </c>
+      <c r="B89" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>92</v>
+      </c>
+      <c r="B90" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>93</v>
+      </c>
+      <c r="B91" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>94</v>
+      </c>
+      <c r="B92" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>95</v>
+      </c>
+      <c r="B93" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>